<commit_message>
Login page test case added.
</commit_message>
<xml_diff>
--- a/TmsAutomation/src/main/resources/testData.xlsx
+++ b/TmsAutomation/src/main/resources/testData.xlsx
@@ -29,14 +29,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -58,6 +60,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,12 +105,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -131,10 +138,10 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.48"/>
@@ -144,7 +151,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="2" t="n">
         <v>1234</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Page Object Model(POM) added
</commit_message>
<xml_diff>
--- a/TmsAutomation/src/main/resources/testData.xlsx
+++ b/TmsAutomation/src/main/resources/testData.xlsx
@@ -20,9 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">admin@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">siloshasilu@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November@1</t>
   </si>
 </sst>
 </file>
@@ -135,13 +141,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.48"/>
@@ -155,9 +161,19 @@
         <v>1234</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="admin@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId2" display="siloshasilu@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId3" display="November@1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>